<commit_message>
fix connector interface test fails
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/sampleTestData.xlsx
+++ b/src/main/resources/test-data-xls/sampleTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B68155F-855D-4907-A1CD-877E3858500A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BC3389-A6F5-4575-8D62-7F4CEEFF3CDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>good request</t>
   </si>
@@ -97,9 +97,6 @@
     <t>bad request (name is empty)</t>
   </si>
   <si>
-    <t>bad request:name cannot be blank!</t>
-  </si>
-  <si>
     <t>bad request (name is not present)</t>
   </si>
   <si>
@@ -109,25 +106,25 @@
     <t>bad request (name does not exist)</t>
   </si>
   <si>
-    <t>entity 12345678 not found locally!</t>
-  </si>
-  <si>
     <t>bad request (name contains strange characters)</t>
   </si>
   <si>
     <t>！@#￥%……&amp;*（）——+？|</t>
   </si>
   <si>
-    <t>entity ！@#￥%……&amp;*（）——+？| not found locally!</t>
-  </si>
-  <si>
     <t>bad request (name is too long)</t>
   </si>
   <si>
     <t>超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024</t>
   </si>
   <si>
-    <t>entity 超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024 not found locally!</t>
+    <t>statusCode</t>
+  </si>
+  <si>
+    <t>searchData.name is not valid,reason: must not be blank</t>
+  </si>
+  <si>
+    <t>The m2 service unavailable: (request M2 failed : no found entity ).</t>
   </si>
 </sst>
 </file>
@@ -583,13 +580,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -606,13 +605,16 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -625,14 +627,14 @@
       <c r="D2">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -645,14 +647,14 @@
       <c r="D3">
         <v>15</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -662,14 +664,14 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -679,14 +681,14 @@
       <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -696,14 +698,14 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -713,14 +715,14 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -730,14 +732,14 @@
       <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -751,32 +753,35 @@
         <v>10</v>
       </c>
       <c r="F9">
+        <v>400</v>
+      </c>
+      <c r="G9">
         <v>106601</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>106602</v>
+      </c>
+      <c r="H10" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>106602</v>
-      </c>
-      <c r="G10" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>26</v>
       </c>
       <c r="B11">
         <v>12345678</v>
@@ -787,54 +792,54 @@
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="F11">
-        <v>106101</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>108001</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>108001</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>106101</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>108001</v>
+      </c>
+      <c r="H13" t="s">
         <v>32</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>106101</v>
-      </c>
-      <c r="G13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -844,10 +849,10 @@
       <c r="E14" t="s">
         <v>12</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>106119</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
iems data-driven test case 1st version
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/sampleTestData.xlsx
+++ b/src/main/resources/test-data-xls/sampleTestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BC3389-A6F5-4575-8D62-7F4CEEFF3CDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C133E8AD-1C69-4835-814C-BFF62709F92F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testDataForMethod1" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchModelDataByCondition" sheetId="2" r:id="rId2"/>
+    <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -459,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -582,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
small refine of code structure
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/sampleTestData.xlsx
+++ b/src/main/resources/test-data-xls/sampleTestData.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C133E8AD-1C69-4835-814C-BFF62709F92F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAEDD2B-679C-4FE1-85AF-D4F5A97AA894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="testDataForMethod1" sheetId="1" r:id="rId1"/>
-    <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId2"/>
+    <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
-  <si>
-    <t>good request</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -49,12 +45,6 @@
     <t>pageSize</t>
   </si>
   <si>
-    <t>expectCode</t>
-  </si>
-  <si>
-    <t>expectMessage</t>
-  </si>
-  <si>
     <t>Operate success.</t>
   </si>
   <si>
@@ -118,20 +108,26 @@
     <t>超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024超长字符1024</t>
   </si>
   <si>
-    <t>statusCode</t>
-  </si>
-  <si>
     <t>searchData.name is not valid,reason: must not be blank</t>
   </si>
   <si>
     <t>The m2 service unavailable: (request M2 failed : no found entity ).</t>
+  </si>
+  <si>
+    <t>rspStatus</t>
+  </si>
+  <si>
+    <t>rspCode</t>
+  </si>
+  <si>
+    <t>rspMessage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,27 +135,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -174,9 +156,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,170 +437,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>106119</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>106119</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>106119</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -631,15 +489,15 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -651,100 +509,100 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -759,12 +617,12 @@
         <v>106601</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -776,12 +634,12 @@
         <v>106602</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>12345678</v>
@@ -796,15 +654,15 @@
         <v>108001</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -816,15 +674,15 @@
         <v>108001</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -836,24 +694,24 @@
         <v>108001</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G14">
         <v>106119</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor xml for executing regression test
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/sampleTestData.xlsx
+++ b/src/main/resources/test-data-xls/sampleTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAEDD2B-679C-4FE1-85AF-D4F5A97AA894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7ABEBF-82DD-403B-8730-D19999838539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -440,11 +440,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
add _in/_nin checking functions
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/sampleTestData.xlsx
+++ b/src/main/resources/test-data-xls/sampleTestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7ABEBF-82DD-403B-8730-D19999838539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853B3642-5376-4723-A472-E2F38943535B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
+    <sheet name="getDataEntities" sheetId="3" r:id="rId2"/>
+    <sheet name="getDataGraphQL" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -121,13 +123,82 @@
   </si>
   <si>
     <t>rspMessage</t>
+  </si>
+  <si>
+    <t>test-id</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>SensorData</t>
+  </si>
+  <si>
+    <t>Successfully</t>
+  </si>
+  <si>
+    <t>iems-api-engine-restful-test-7</t>
+  </si>
+  <si>
+    <t>iems-api-engine-restful-test-8</t>
+  </si>
+  <si>
+    <t>iems-api-engine-restful-test-9</t>
+  </si>
+  <si>
+    <t>[SensorData][][][updateTime asc][1,10]</t>
+  </si>
+  <si>
+    <t>iems-api-engine-restful-test-10</t>
+  </si>
+  <si>
+    <t>[SensorData][][][updateTime dsc][1,15]</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>iems-api-engine-graphql-test-5</t>
+  </si>
+  <si>
+    <t>bad request</t>
+  </si>
+  <si>
+    <t>{SensorData(cond:"{Siid: {_invalid: 999999}}")  {Siid type value}}</t>
+  </si>
+  <si>
+    <t>can not parse _invalid: 999999</t>
+  </si>
+  <si>
+    <t>iems-api-engine-graphql-test-6</t>
+  </si>
+  <si>
+    <t>{SensorData(cond:"{Siid: {_in: [5040, 5045, 34155]}}") {Siid type value}}</t>
+  </si>
+  <si>
+    <t>[SensorData][type,Siid][{Siid: {_in: [5040, 5045, 34155]}}][][]</t>
+  </si>
+  <si>
+    <t>[SensorData][type,Siid][{Siid: {_nin: [5040, 5045, 34155]}}][][]</t>
+  </si>
+  <si>
+    <t>iems-api-engine-graphql-test-7</t>
+  </si>
+  <si>
+    <t>{SensorData(cond:"{Siid: {_nin: [5040, 5045, 34155]}}") {Siid type value}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,16 +206,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,12 +242,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -721,4 +829,252 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1143CFE-9DFF-4D3E-BF65-C106E67B4F3A}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" style="2"/>
+    <col min="4" max="4" width="36.6328125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="12.6328125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3">
+        <v>200</v>
+      </c>
+      <c r="G3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3">
+        <v>200</v>
+      </c>
+      <c r="G4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3">
+        <v>200</v>
+      </c>
+      <c r="G5" s="3">
+        <v>100000</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24431FB0-2102-4F18-A28E-FB863336562B}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="60.6328125" style="2" customWidth="1"/>
+    <col min="4" max="6" width="12.6328125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="3">
+        <v>200</v>
+      </c>
+      <c r="E2" s="3">
+        <v>101302</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="3">
+        <v>200</v>
+      </c>
+      <c r="E4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add entity management test case, 1st batch
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/sampleTestData.xlsx
+++ b/src/main/resources/test-data-xls/sampleTestData.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4914B54-FEC4-4DCE-B457-BDF0A0DA583F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD6ECC0-F919-47B2-B613-2E6B4A00BE1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition-" sheetId="2" r:id="rId1"/>
     <sheet name="getDataEntities-iems" sheetId="3" r:id="rId2"/>
     <sheet name="getDataGraphQL-iems" sheetId="4" r:id="rId3"/>
     <sheet name="getDataGraphQL" sheetId="5" r:id="rId4"/>
+    <sheet name="createEntityInDomain" sheetId="7" r:id="rId5"/>
+    <sheet name="updateEntity" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
   <si>
     <t>name</t>
   </si>
@@ -223,6 +225,30 @@
   </si>
   <si>
     <t>{Project(cond:"{_or: [{business_mgr:{_in:[\"潘云晖\",\"臧佳宝\" ]}},{status:{_in:[\"archived\" ]}}]}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status  invert_Customer (cond:"{id:{_eq:24}}",order:"") {actual_controller category cid city cname contact contact_detail ctype district enterprise_size group holding_type id is_connected_tx is_gov_fin_customer is_group_customer legal_person legal_person_id major_class middle_class office_address project province registered_address small_class}}}</t>
+  </si>
+  <si>
+    <t>good request</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>SNC</t>
+  </si>
+  <si>
+    <t>testEntity1</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>{"id":"41","label":"Device","properties":{"metadata_node_type":"entity","metadata_node_domain":"SNC","additional_prop1":"value1","additional_prop2":"value2"},"nodeType":"ENTITY","location":"SNC"}</t>
   </si>
 </sst>
 </file>
@@ -292,11 +318,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,12 +612,12 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -614,7 +643,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -634,7 +663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -654,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -671,7 +700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -688,7 +717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -705,7 +734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -722,7 +751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -739,7 +768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -762,7 +791,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -779,7 +808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -799,7 +828,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -819,7 +848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -839,7 +868,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -871,15 +900,15 @@
       <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="2"/>
-    <col min="4" max="4" width="36.5703125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="12.5703125" style="2"/>
+    <col min="1" max="2" width="30.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="2"/>
+    <col min="4" max="4" width="36.54296875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="12.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -905,7 +934,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -929,7 +958,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -953,7 +982,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -977,7 +1006,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
@@ -1015,15 +1044,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" style="2" customWidth="1"/>
-    <col min="4" max="6" width="12.5703125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="2" width="30.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="60.54296875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="12.54296875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1043,7 +1072,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1063,7 +1092,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -1083,7 +1112,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -1114,19 +1143,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6671BC86-BAF8-4F8B-AA39-F1BCADD8DBDD}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" style="2" customWidth="1"/>
-    <col min="4" max="6" width="12.5703125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="2" width="30.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="60.54296875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="12.54296875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1146,7 +1175,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>61</v>
       </c>
@@ -1166,7 +1195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
@@ -1186,7 +1215,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>55</v>
       </c>
@@ -1206,7 +1235,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>57</v>
       </c>
@@ -1226,7 +1255,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>59</v>
       </c>
@@ -1244,6 +1273,145 @@
       </c>
       <c r="F6" s="3" t="s">
         <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEE90B5-8324-4382-A812-BC38A40E26FE}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.54296875" style="2" customWidth="1"/>
+    <col min="3" max="4" width="16.6328125" style="2" customWidth="1"/>
+    <col min="5" max="7" width="12.54296875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2E6211-E3DA-4C96-96F7-EC9288FA6A46}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.54296875" style="2" customWidth="1"/>
+    <col min="3" max="4" width="16.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.6328125" style="2" customWidth="1"/>
+    <col min="6" max="8" width="12.54296875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3">
+        <v>200</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add entity management test case, 2nd batch
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/sampleTestData.xlsx
+++ b/src/main/resources/test-data-xls/sampleTestData.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD6ECC0-F919-47B2-B613-2E6B4A00BE1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9DCAE7-B5C9-49C8-9143-4C8613DAA8D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition-" sheetId="2" r:id="rId1"/>
     <sheet name="getDataEntities-iems" sheetId="3" r:id="rId2"/>
     <sheet name="getDataGraphQL-iems" sheetId="4" r:id="rId3"/>
     <sheet name="getDataGraphQL" sheetId="5" r:id="rId4"/>
-    <sheet name="createEntityInDomain" sheetId="7" r:id="rId5"/>
-    <sheet name="updateEntity" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
   <si>
     <t>name</t>
   </si>
@@ -225,30 +223,6 @@
   </si>
   <si>
     <t>{Project(cond:"{_or: [{business_mgr:{_in:[\"潘云晖\",\"臧佳宝\" ]}},{status:{_in:[\"archived\" ]}}]}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status  invert_Customer (cond:"{id:{_eq:24}}",order:"") {actual_controller category cid city cname contact contact_detail ctype district enterprise_size group holding_type id is_connected_tx is_gov_fin_customer is_group_customer legal_person legal_person_id major_class middle_class office_address project province registered_address small_class}}}</t>
-  </si>
-  <si>
-    <t>good request</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>entity</t>
-  </si>
-  <si>
-    <t>SNC</t>
-  </si>
-  <si>
-    <t>testEntity1</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>{"id":"41","label":"Device","properties":{"metadata_node_type":"entity","metadata_node_domain":"SNC","additional_prop1":"value1","additional_prop2":"value2"},"nodeType":"ENTITY","location":"SNC"}</t>
   </si>
 </sst>
 </file>
@@ -318,14 +292,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1143CFE-9DFF-4D3E-BF65-C106E67B4F3A}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
@@ -1279,143 +1250,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEE90B5-8324-4382-A812-BC38A40E26FE}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="30.54296875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="16.6328125" style="2" customWidth="1"/>
-    <col min="5" max="7" width="12.54296875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="3">
-        <v>200</v>
-      </c>
-      <c r="F2" s="3">
-        <v>200</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2E6211-E3DA-4C96-96F7-EC9288FA6A46}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="30.54296875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="16.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="36.6328125" style="2" customWidth="1"/>
-    <col min="6" max="8" width="12.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="3">
-        <v>200</v>
-      </c>
-      <c r="G2" s="3">
-        <v>200</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>